<commit_message>
proof of concept - fed instead of state data
</commit_message>
<xml_diff>
--- a/test-data/expected_result_postcode_state.xlsx
+++ b/test-data/expected_result_postcode_state.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JakeClarke\source\personalprojects\geography-weighter\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D29E25C-D24F-49FF-A316-9891ABD69C66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A49E990-0B2D-4242-A498-429E96BE4709}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4140" yWindow="4140" windowWidth="28800" windowHeight="15560" xr2:uid="{95D972A8-8080-424A-8D3E-D20917D58757}"/>
   </bookViews>
@@ -423,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5F0C2A4-48CA-4F99-85D5-84C3F1C8CEB3}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -442,7 +442,7 @@
     <col min="9" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,7 +468,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>3003</v>
       </c>
@@ -498,7 +498,7 @@
         <v>124.956</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>3004</v>
       </c>
@@ -528,7 +528,7 @@
         <v>1619.2701</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3006</v>
       </c>
@@ -558,7 +558,7 @@
         <v>17996</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3008</v>
       </c>
@@ -588,7 +588,7 @@
         <v>2259.5936999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>3182</v>
       </c>
@@ -618,7 +618,7 @@
         <v>16655.063400000003</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>3205</v>
       </c>
@@ -648,7 +648,7 @@
         <v>10317</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>3206</v>
       </c>
@@ -678,7 +678,7 @@
         <v>9699</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>3207</v>
       </c>
@@ -708,7 +708,7 @@
         <v>15348</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F11" s="1">
         <f>SUM(F2:F9)</f>
         <v>77983.481400000004</v>
@@ -716,6 +716,10 @@
       <c r="H11" s="1">
         <f>SUM(H1:H9)</f>
         <v>74018.883200000011</v>
+      </c>
+      <c r="J11" s="1">
+        <f>H11/F11</f>
+        <v>0.94916105143261797</v>
       </c>
     </row>
   </sheetData>

</xml_diff>